<commit_message>
Simple mistake in managing the colors in multicolor modes char and bitmap.
</commit_message>
<xml_diff>
--- a/docs/Binary.xlsx
+++ b/docs/Binary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkspacesII\EMULATORS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F6BFDF4-D12F-49CB-B73F-F491E6A2B8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AF87DE-48E1-4068-8A9B-9D8A3628328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{16126F91-A69E-43AB-A1DA-EEABA66B40FE}"/>
   </bookViews>
@@ -46,12 +46,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +78,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,86 +399,91 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="3" width="10.9453125" style="1"/>
+    <col min="4" max="4" width="14.89453125" style="1" customWidth="1"/>
+    <col min="5" max="8" width="10.9453125" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>7</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>6</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>5</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>4</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="2">
         <v>3</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="2">
         <v>2</v>
       </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
+      <c r="G1" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>128</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>64</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>32</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>16</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>8</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>4</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
         <v>1</v>
       </c>
       <c r="I3">
@@ -477,15 +496,56 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
       <c r="I4">
         <f t="shared" ref="I4:I10" si="0">A4*A$2+B4*B$2+C4*C$2+D4*D$2+E4*E$2+F4*F$2+G4*G$2+H4*H$2</f>
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J10" si="1">DEC2HEX(I4)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v>1C</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -493,28 +553,48 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="I7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="I8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="I9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="I10">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>